<commit_message>
Start making dialogue generator
</commit_message>
<xml_diff>
--- a/src/events.xlsx
+++ b/src/events.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\azulon\cluedo\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACABCC6-2331-4D64-9CB8-E301D64D80C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D8C72A-39C1-4B8E-BE97-23BC02BA0961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -720,9 +720,6 @@
     <t>When the OPTION is clicked, advance to the FRAME with this ID.</t>
   </si>
   <si>
-    <t>The LINE will only appear if this condition is met. Ensure that an OPTION will always appear, regardless of variable status.</t>
-  </si>
-  <si>
     <t>If this is the last LINE of the FRAME, these OPTIONS will appear. If blank, there will be a single "Next" option.</t>
   </si>
   <si>
@@ -776,6 +773,9 @@
     <t xml:space="preserve">"We know //how// and //where//. What question remains?
 We need the //who//. And //why//, if it's not inane."
 </t>
+  </si>
+  <si>
+    <t>The OPTION will only appear if this condition is met. If a LINE has no options that will appear, it will not appear at all.</t>
   </si>
 </sst>
 </file>
@@ -928,13 +928,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -945,7 +945,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{8217AA4A-92D9-4D13-A3BC-71C24F941B31}"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -971,104 +971,6 @@
       <fill>
         <patternFill>
           <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFECF4FA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFAEB"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1392,10 +1294,10 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D100" sqref="D100"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -1404,8 +1306,8 @@
     <col min="2" max="2" width="19.88671875" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="61.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="38.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="32.88671875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.88671875" style="2" customWidth="1"/>
     <col min="7" max="7" width="22.77734375" style="1" customWidth="1"/>
     <col min="8" max="8" width="6.77734375" style="4" customWidth="1"/>
     <col min="9" max="11" width="25.88671875" style="1" customWidth="1"/>
@@ -1425,11 +1327,11 @@
       <c r="D1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>1</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>2</v>
@@ -1447,30 +1349,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="13" customFormat="1" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="11" customFormat="1" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="F2" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="11" t="s">
+        <v>181</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>167</v>
       </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
     </row>
     <row r="3" spans="1:11" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
@@ -1514,7 +1416,7 @@
         <v>32</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>25</v>
@@ -1577,7 +1479,7 @@
       <c r="D16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>112</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1588,7 +1490,7 @@
       <c r="D17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>113</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1599,7 +1501,7 @@
       <c r="D18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>114</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1610,7 +1512,7 @@
       <c r="D19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>115</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1621,7 +1523,7 @@
       <c r="D20" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>116</v>
       </c>
       <c r="G20" s="1" t="s">
@@ -1632,7 +1534,7 @@
       <c r="D21" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>117</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -1649,13 +1551,13 @@
       <c r="D22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" ht="69" x14ac:dyDescent="0.3">
       <c r="D23" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1666,7 +1568,7 @@
       <c r="D24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1674,7 +1576,7 @@
       <c r="D25" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="F25" s="2" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1685,7 +1587,7 @@
       <c r="D26" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="F26" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1693,7 +1595,7 @@
       <c r="D27" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>126</v>
       </c>
     </row>
@@ -1704,7 +1606,7 @@
       <c r="D28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="F28" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1712,7 +1614,7 @@
       <c r="D29" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="F29" s="2" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1723,7 +1625,7 @@
       <c r="D30" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="F30" s="2" t="s">
         <v>131</v>
       </c>
     </row>
@@ -1734,7 +1636,7 @@
       <c r="D31" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="F31" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -1745,11 +1647,11 @@
       <c r="D32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="F32" s="2" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>137</v>
       </c>
@@ -1760,20 +1662,20 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="D34" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="41.4" x14ac:dyDescent="0.3">
       <c r="D35" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>140</v>
       </c>
@@ -1781,12 +1683,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D37" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>143</v>
       </c>
@@ -1797,12 +1699,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D39" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>144</v>
       </c>
@@ -1810,17 +1712,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D41" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D42" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>145</v>
       </c>
@@ -1828,17 +1730,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D44" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D45" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>146</v>
       </c>
@@ -1846,12 +1748,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D47" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D48" s="3" t="s">
         <v>59</v>
       </c>
@@ -1897,7 +1799,7 @@
         <v>149</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
@@ -1955,7 +1857,7 @@
     </row>
     <row r="63" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D63" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
@@ -1969,17 +1871,17 @@
         <v>73</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D65" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D66" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>158</v>
       </c>
@@ -1990,12 +1892,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D68" s="3" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>160</v>
       </c>
@@ -2003,74 +1905,74 @@
         <v>87</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D70" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
       <c r="D71" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D72" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="D73" s="3" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
       <c r="D74" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D75" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D76" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F76" s="1" t="s">
+      <c r="E76" s="1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D77" s="3"/>
-      <c r="F77" s="1" t="s">
+      <c r="E77" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
       <c r="D78" s="3"/>
-      <c r="F78" s="1" t="s">
+      <c r="E78" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D79" s="3"/>
-      <c r="F79" s="1" t="s">
+      <c r="E79" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D80" s="3"/>
-      <c r="F80" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D81" s="3"/>
-      <c r="F81" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2084,7 +1986,7 @@
       <c r="D82" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2092,7 +1994,7 @@
       <c r="D83" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E83" s="2" t="s">
+      <c r="F83" s="2" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2100,7 +2002,7 @@
       <c r="D84" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E84" s="2" t="s">
+      <c r="F84" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2108,7 +2010,7 @@
       <c r="D85" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="E85" s="2" t="s">
+      <c r="F85" s="2" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2116,7 +2018,7 @@
       <c r="D86" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="F86" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2124,7 +2026,7 @@
       <c r="D87" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E87" s="2" t="s">
+      <c r="F87" s="2" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2132,7 +2034,7 @@
       <c r="D88" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="E88" s="2" t="s">
+      <c r="F88" s="2" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2140,7 +2042,7 @@
       <c r="D89" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E89" s="2" t="s">
+      <c r="F89" s="2" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2148,7 +2050,7 @@
       <c r="D90" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E90" s="2" t="s">
+      <c r="F90" s="2" t="s">
         <v>118</v>
       </c>
     </row>
@@ -2170,39 +2072,39 @@
     </row>
     <row r="93" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D93" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D94" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="E94" s="2" t="s">
-        <v>180</v>
+        <v>176</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="95" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D95" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="E95" s="2" t="s">
-        <v>180</v>
+      <c r="F95" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="96" spans="1:6" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D96" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E96" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="97" spans="4:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="D97" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="98" spans="4:4" ht="41.4" x14ac:dyDescent="0.25">

</xml_diff>